<commit_message>
3 cart selections done
</commit_message>
<xml_diff>
--- a/npcs/Food Cart Stock.xlsx
+++ b/npcs/Food Cart Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d272a33b67c842f2/Desktop/shocked-anguilliform.github.io/npcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6298F04-DFF6-46BC-B9FC-5BB2A4485080}"/>
+  <xr:revisionPtr revIDLastSave="320" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{239736C1-EFEB-4905-B608-287967859159}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="1065" windowWidth="15375" windowHeight="8325" xr2:uid="{D64F0F03-2BA3-4991-A974-0C211D30659A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>Popcorn</t>
   </si>
@@ -299,7 +299,52 @@
     <t>Stock is consistent (except for candied fruits that rotate weekly). This is the menu.</t>
   </si>
   <si>
-    <t>Ham and Cheese</t>
+    <t>Every order comes in a light waffle bowl with a waffle spoon.</t>
+  </si>
+  <si>
+    <t>Bacon &amp; Pineapple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomatosala </t>
+  </si>
+  <si>
+    <t>Garlic &amp; Herb Cheese</t>
+  </si>
+  <si>
+    <t>(tomato, onion, spices)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garden Bounty </t>
+  </si>
+  <si>
+    <t>(different veggie mix every week)</t>
+  </si>
+  <si>
+    <t>Ham &amp; Cheese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ginger Duck </t>
+  </si>
+  <si>
+    <t>Amaranth &amp; Mushroom</t>
+  </si>
+  <si>
+    <t>Caramel Banana</t>
+  </si>
+  <si>
+    <t>Lemon Coconut</t>
+  </si>
+  <si>
+    <t>Honey Nut</t>
+  </si>
+  <si>
+    <t>Seaside (fish, leek, dill)</t>
+  </si>
+  <si>
+    <t>Strawberry Cocoplum</t>
+  </si>
+  <si>
+    <t>Pomegranate Fig Ricotta</t>
   </si>
 </sst>
 </file>
@@ -365,14 +410,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3B16E-7656-4A12-AA96-94DC10DCD96A}">
-  <dimension ref="A2:I70"/>
+  <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,368 +1144,425 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A33" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="H34" s="3" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="H35" s="3" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="H35" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
       <c r="H36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
       <c r="H37" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="I37" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="H38" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" t="s">
-        <v>55</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>14</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>15</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>16</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>17</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>18</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>19</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>20</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="58" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="3" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>92</v>
+      </c>
+      <c r="E62" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="E65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D67" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D65">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68">
         <v>1</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E68" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D66">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69">
         <v>2</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D67">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70">
         <v>3</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E70" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D68">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D71">
         <v>4</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E71" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D69">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72">
         <v>5</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E72" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D70">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D73">
         <v>6</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E73" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C56:E56"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C55:E55"/>
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C44:E44"/>
     <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
lots of lil changes but now im tired
</commit_message>
<xml_diff>
--- a/npcs/Food Cart Stock.xlsx
+++ b/npcs/Food Cart Stock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d272a33b67c842f2/Desktop/shocked-anguilliform.github.io/npcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="912" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E948D5E-17A1-4FA0-B2C7-1E095935580B}"/>
+  <xr:revisionPtr revIDLastSave="1021" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F91177-C054-4F41-BC89-6EE5A2532470}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="690" windowWidth="14985" windowHeight="8325" xr2:uid="{D64F0F03-2BA3-4991-A974-0C211D30659A}"/>
+    <workbookView xWindow="9825" yWindow="2175" windowWidth="15375" windowHeight="8325" xr2:uid="{D64F0F03-2BA3-4991-A974-0C211D30659A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="241">
   <si>
     <t>Popcorn</t>
   </si>
@@ -651,9 +651,6 @@
     <t>(lots of cheese, onion (pizza w/o marrinara sauce))</t>
   </si>
   <si>
-    <t>(mixed grill style roast fish, sika deer, duck, iguana)</t>
-  </si>
-  <si>
     <t>House Dishes</t>
   </si>
   <si>
@@ -675,9 +672,6 @@
     <t>big enough for an entire dorm house or study group. Has a very homely &amp; boisterous atmosphere.</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guava Citrus Kombucha  </t>
   </si>
   <si>
@@ -691,6 +685,129 @@
   </si>
   <si>
     <t xml:space="preserve">Drinks (V)                              </t>
+  </si>
+  <si>
+    <t>(mixed grill style roast fish, antelope, duck, iguana)</t>
+  </si>
+  <si>
+    <t>Saltenas</t>
+  </si>
+  <si>
+    <t>(varying meat &amp; veg, scrambled eggs, chayote squash, onions)</t>
+  </si>
+  <si>
+    <t>Sfenj</t>
+  </si>
+  <si>
+    <t>(donut thing with powdered sugar, honey, topped with varying fruit)</t>
+  </si>
+  <si>
+    <t>Morning Glories</t>
+  </si>
+  <si>
+    <t>Coffee Bar</t>
+  </si>
+  <si>
+    <t>(cookies with cinnamon, ginger, papaya, cherimoya, coconut, walnuts)</t>
+  </si>
+  <si>
+    <t>Jumble Bread</t>
+  </si>
+  <si>
+    <t>(packed with different ingredients every day- can be herbs, nuts, fruits, maybe veggies)</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Cafe Hall</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Breakfast Spread</t>
+  </si>
+  <si>
+    <t>Tacos</t>
+  </si>
+  <si>
+    <t>Salad Wrap</t>
+  </si>
+  <si>
+    <t>Island Salad</t>
+  </si>
+  <si>
+    <t>(red amaranth leaves mixed with varying foraged leaves and toppings)</t>
+  </si>
+  <si>
+    <t>(crowder peas, red amaranth, tomatillos, yellow squash, onion)</t>
+  </si>
+  <si>
+    <t>(all able to be taken to go)</t>
+  </si>
+  <si>
+    <t>Meat &amp; Rice</t>
+  </si>
+  <si>
+    <t>(could be curry, stewed meat, rendang, paella, depends on the meat)</t>
+  </si>
+  <si>
+    <t>Hot Pot</t>
+  </si>
+  <si>
+    <t>Fried Bananas</t>
+  </si>
+  <si>
+    <t>(often corbasi (yogurt or lentil soup) sometimes a stew, soup)</t>
+  </si>
+  <si>
+    <t>(varying meat and veggies, herbs, cheese) (usually birria, sometimes spit roast))</t>
+  </si>
+  <si>
+    <t>Stuffed Stuff</t>
+  </si>
+  <si>
+    <t>(stuffed veggies, meat pies, risoles (basically breaded and fried burritoes), fritters, croquettes, etc…)</t>
+  </si>
+  <si>
+    <t>Friday Special</t>
+  </si>
+  <si>
+    <t>(whatever the kitchen feels like making that day- sometimes something the head chef hunted themselves)</t>
+  </si>
+  <si>
+    <t>Chocotorta</t>
+  </si>
+  <si>
+    <t>Chilenitos</t>
+  </si>
+  <si>
+    <t>Mango Mousse</t>
+  </si>
+  <si>
+    <t>1d4</t>
+  </si>
+  <si>
+    <t>The food served changes by the day (besides a few staples). Vegan variations are available for</t>
+  </si>
+  <si>
+    <t>every dish served (except desserts made with eggs).</t>
+  </si>
+  <si>
+    <t>(wafer cookies sandwiching dulce de leche and covered in meringue)</t>
+  </si>
+  <si>
+    <t>(chocolate, coffee, cream, dulce de leche cake)</t>
   </si>
 </sst>
 </file>
@@ -769,10 +886,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1089,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3B16E-7656-4A12-AA96-94DC10DCD96A}">
-  <dimension ref="A2:K128"/>
+  <dimension ref="A2:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1609,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1512,9 +1629,9 @@
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -1526,9 +1643,9 @@
       <c r="B35" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
       <c r="H35" s="3" t="s">
         <v>62</v>
       </c>
@@ -1541,9 +1658,9 @@
       <c r="B36" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
       <c r="H36" t="s">
         <v>63</v>
       </c>
@@ -1558,9 +1675,9 @@
       <c r="B37" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
       <c r="H37" t="s">
         <v>64</v>
       </c>
@@ -1575,9 +1692,9 @@
       <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
       <c r="H38" s="6" t="s">
         <v>112</v>
       </c>
@@ -1606,9 +1723,9 @@
       <c r="B40" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
       <c r="H40" s="8" t="s">
         <v>124</v>
       </c>
@@ -1620,9 +1737,9 @@
       <c r="B41" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1631,9 +1748,9 @@
       <c r="B42" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -1642,9 +1759,9 @@
       <c r="B43" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -1653,9 +1770,9 @@
       <c r="B44" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -1675,9 +1792,9 @@
       <c r="B46" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -1686,9 +1803,9 @@
       <c r="B47" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -1708,9 +1825,9 @@
       <c r="B49" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -1719,9 +1836,9 @@
       <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
@@ -1730,9 +1847,9 @@
       <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -1741,9 +1858,9 @@
       <c r="B52" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -1752,9 +1869,9 @@
       <c r="B53" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -1763,9 +1880,9 @@
       <c r="B54" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -1774,14 +1891,14 @@
       <c r="B55" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
@@ -2203,12 +2320,12 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -2216,13 +2333,13 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>185</v>
@@ -2283,7 +2400,7 @@
         <v>157</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="E116" s="4"/>
     </row>
@@ -2292,10 +2409,10 @@
         <v>171</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -2306,7 +2423,7 @@
         <v>170</v>
       </c>
       <c r="H119" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -2329,7 +2446,7 @@
         <v>166</v>
       </c>
       <c r="H121" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -2351,7 +2468,7 @@
         <v>168</v>
       </c>
       <c r="H123" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -2362,30 +2479,205 @@
         <v>169</v>
       </c>
       <c r="H124" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H125" s="10"/>
-      <c r="I125" s="10"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="9"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>196</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B133" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>201</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>205</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>215</v>
+      </c>
+      <c r="B139" t="s">
+        <v>203</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B141" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>219</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>218</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>212</v>
+      </c>
+      <c r="B144" t="s">
+        <v>225</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>213</v>
+      </c>
+      <c r="B145" t="s">
+        <v>217</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>214</v>
+      </c>
+      <c r="B146" t="s">
+        <v>223</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>213</v>
+      </c>
+      <c r="B147" t="s">
+        <v>229</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>215</v>
+      </c>
+      <c r="B148" t="s">
+        <v>231</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>234</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>3</v>
+      </c>
+      <c r="B153" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>4</v>
+      </c>
+      <c r="B154" t="s">
+        <v>233</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="C50:E50"/>
@@ -2402,6 +2694,11 @@
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Hwen more prepared... tired now
</commit_message>
<xml_diff>
--- a/npcs/Food Cart Stock.xlsx
+++ b/npcs/Food Cart Stock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d272a33b67c842f2/Desktop/shocked-anguilliform.github.io/npcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1047" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24DF5913-EB8E-45CD-A44C-ACF00465CC30}"/>
+  <xr:revisionPtr revIDLastSave="1048" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B2E0BF-D590-4A8F-AB70-F49C206E2FBA}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="15375" windowHeight="8325" xr2:uid="{D64F0F03-2BA3-4991-A974-0C211D30659A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="245">
   <si>
     <t>Popcorn</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>Kebabs</t>
-  </si>
-  <si>
-    <t>(kebab cart)</t>
   </si>
   <si>
     <t>Sides</t>
@@ -1217,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3B16E-7656-4A12-AA96-94DC10DCD96A}">
   <dimension ref="A2:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="J149" sqref="J149"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1618,7 +1615,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1701,7 +1698,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="H38" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1715,10 +1712,10 @@
         <v>45</v>
       </c>
       <c r="H39" t="s">
+        <v>121</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1732,7 +1729,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="H40" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1952,7 +1949,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E65" t="s">
         <v>83</v>
@@ -2037,17 +2034,17 @@
     </row>
     <row r="76" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2063,100 +2060,100 @@
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G81">
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G82">
         <v>2</v>
       </c>
       <c r="H82" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G83">
         <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G84">
         <v>4</v>
       </c>
       <c r="H84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G85">
         <v>5</v>
       </c>
       <c r="H85" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="G86">
         <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G87">
         <v>7</v>
       </c>
       <c r="H87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -2164,98 +2161,98 @@
         <v>8</v>
       </c>
       <c r="H88" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G89">
         <v>9</v>
       </c>
       <c r="H89" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C90" s="4"/>
       <c r="G90">
         <v>10</v>
       </c>
       <c r="H90" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>114</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G91">
         <v>11</v>
       </c>
       <c r="H91" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G92">
         <v>12</v>
       </c>
       <c r="H92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G93">
         <v>13</v>
       </c>
       <c r="H93" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G94">
         <v>14</v>
       </c>
       <c r="H94" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C95" s="4"/>
       <c r="G95">
         <v>15</v>
       </c>
       <c r="H95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
@@ -2263,46 +2260,46 @@
         <v>16</v>
       </c>
       <c r="H96" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G97">
         <v>17</v>
       </c>
       <c r="H97" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
+        <v>124</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="G98">
         <v>18</v>
       </c>
       <c r="H98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
+        <v>146</v>
+      </c>
+      <c r="C99" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="G99">
         <v>19</v>
       </c>
       <c r="H99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -2310,27 +2307,27 @@
         <v>20</v>
       </c>
       <c r="H100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -2338,150 +2335,150 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H107" s="1"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
+        <v>160</v>
+      </c>
+      <c r="D114" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E118" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H118" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E119" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H119" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C120" s="4"/>
       <c r="E120" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H120" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E121" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H121" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E122" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H122" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E123" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H123" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -2490,51 +2487,51 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C133" s="4"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B136" t="s">
         <v>50</v>
@@ -2542,135 +2539,135 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
+        <v>199</v>
+      </c>
+      <c r="C139" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
+        <v>206</v>
+      </c>
+      <c r="C140" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B142" t="s">
+        <v>201</v>
+      </c>
+      <c r="C142" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
+        <v>217</v>
+      </c>
+      <c r="C145" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B147" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B148" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B149" t="s">
+        <v>221</v>
+      </c>
+      <c r="C149" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B150" t="s">
+        <v>226</v>
+      </c>
+      <c r="C150" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B151" t="s">
+        <v>228</v>
+      </c>
+      <c r="C151" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2678,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,10 +2683,10 @@
         <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2697,7 +2694,7 @@
         <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2705,24 +2702,19 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="C50:E50"/>
@@ -2739,6 +2731,11 @@
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
tweaks and descriptive text
</commit_message>
<xml_diff>
--- a/npcs/Food Cart Stock.xlsx
+++ b/npcs/Food Cart Stock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d272a33b67c842f2/Desktop/shocked-anguilliform.github.io/npcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1048" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B2E0BF-D590-4A8F-AB70-F49C206E2FBA}"/>
+  <xr:revisionPtr revIDLastSave="1100" documentId="8_{0A2E2A70-4F97-41B1-80B2-89E0A1A7C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F77E9A4A-C815-4318-80E0-0E725939AF21}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="15375" windowHeight="8325" xr2:uid="{D64F0F03-2BA3-4991-A974-0C211D30659A}"/>
+    <workbookView xWindow="2970" yWindow="1635" windowWidth="15375" windowHeight="8325" xr2:uid="{D64F0F03-2BA3-4991-A974-0C211D30659A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="246">
   <si>
     <t>Popcorn</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Helado</t>
   </si>
   <si>
-    <t>(helado cart)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Roll for flavors each week when inquired. On tables for two flavors, Randall either </t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>1d10</t>
   </si>
   <si>
-    <t>(crepe cart)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Savory Crepes </t>
   </si>
   <si>
@@ -262,9 +256,6 @@
     <t>Strawberries</t>
   </si>
   <si>
-    <t>Cherimoya Slices</t>
-  </si>
-  <si>
     <t>Goumi Berries</t>
   </si>
   <si>
@@ -352,16 +343,7 @@
     <t>Dray's Quarry</t>
   </si>
   <si>
-    <t>Ragin Boar</t>
-  </si>
-  <si>
     <t>Catch of the Day</t>
-  </si>
-  <si>
-    <t>(spiced boar, yellow squash, onion, jalapeno)</t>
-  </si>
-  <si>
-    <t>(daily catch and couple veggies)</t>
   </si>
   <si>
     <t>(chayote, eggplant, poblanos, shrooms, garlic)</t>
@@ -398,9 +380,6 @@
     </r>
   </si>
   <si>
-    <t>(pineapple, mango, watermelon, chili, honey)</t>
-  </si>
-  <si>
     <t>(mahi-mahi, pineapple, tomatilloes, peppers)</t>
   </si>
   <si>
@@ -452,16 +431,10 @@
     <t>Bluefin Trevally</t>
   </si>
   <si>
-    <t>Cobia</t>
-  </si>
-  <si>
     <t>Mackerel</t>
   </si>
   <si>
     <t>Marlin</t>
-  </si>
-  <si>
-    <t>Opah</t>
   </si>
   <si>
     <t>Sailfish</t>
@@ -654,12 +627,6 @@
     <t>Hot Curry (V*)</t>
   </si>
   <si>
-    <t>Desserts (V)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (V) = Vegetarian or *alternative available | Everything can be ordered in single and group sizes</t>
-  </si>
-  <si>
     <t xml:space="preserve">  *Center Spice is cinnamon with exotic spices</t>
   </si>
   <si>
@@ -702,9 +669,6 @@
     <t>Coffee Bar</t>
   </si>
   <si>
-    <t>(cookies with cinnamon, ginger, papaya, cherimoya, coconut, walnuts)</t>
-  </si>
-  <si>
     <t>Jumble Bread</t>
   </si>
   <si>
@@ -714,9 +678,6 @@
     <t>Lunch</t>
   </si>
   <si>
-    <t>Cafe Hall</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -744,9 +705,6 @@
     <t>(red amaranth leaves mixed with varying foraged leaves and toppings)</t>
   </si>
   <si>
-    <t>(crowder peas, red amaranth, tomatillos, yellow squash, onion)</t>
-  </si>
-  <si>
     <t>(all able to be taken to go)</t>
   </si>
   <si>
@@ -820,6 +778,63 @@
   </si>
   <si>
     <t>(varying meat and veggies, herbs, cheese (usually birria, sometimes spit roast))</t>
+  </si>
+  <si>
+    <t>Pineapple Rings</t>
+  </si>
+  <si>
+    <t>(daily catch and a couple veggies)</t>
+  </si>
+  <si>
+    <t>Ragin Warthog</t>
+  </si>
+  <si>
+    <t>(spiced ham, yellow squash, onion, jalapeno)</t>
+  </si>
+  <si>
+    <t>(pineapple, peach, watermelon, chili, honey)</t>
+  </si>
+  <si>
+    <t>Octopus</t>
+  </si>
+  <si>
+    <t>Lobster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (V) = Vegetarian   (V*) = Vegetarian alternative available  |  Everything can be ordered in single and group sizes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Desserts (V) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(one prepped daily)</t>
+    </r>
+  </si>
+  <si>
+    <t>M-T</t>
+  </si>
+  <si>
+    <t>(crowder peas, red amaranth, tomatillos, yellow squash, onion) (version with meat from daily caught game as well)</t>
+  </si>
+  <si>
+    <t>(thick cookies with cinnamon, ginger, papaya, cherimoya, coconut, walnuts)</t>
+  </si>
+  <si>
+    <t>Dining Hall</t>
+  </si>
+  <si>
+    <t>Golden Griddle</t>
+  </si>
+  <si>
+    <t>Snow Grove</t>
   </si>
 </sst>
 </file>
@@ -890,13 +905,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,6 +928,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1214,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3B16E-7656-4A12-AA96-94DC10DCD96A}">
   <dimension ref="A2:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +1262,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1265,7 +1284,7 @@
         <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>25</v>
@@ -1284,13 +1303,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1304,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -1344,13 +1363,13 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10">
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1370,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1384,7 +1403,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12">
         <v>6</v>
@@ -1404,13 +1423,13 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13">
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1424,13 +1443,13 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14">
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1470,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,7 +1503,7 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1540,7 +1559,7 @@
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1554,7 +1573,7 @@
         <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,7 +1587,7 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,7 +1615,7 @@
         <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,29 +1633,29 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>191</v>
+      <c r="A28" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1645,11 +1664,11 @@
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
       <c r="H35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K35" s="1"/>
     </row>
@@ -1658,16 +1677,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
       <c r="H36" t="s">
-        <v>63</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1675,16 +1694,16 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
       <c r="H37" t="s">
-        <v>64</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1694,11 +1713,11 @@
       <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="H38" s="4" t="s">
-        <v>111</v>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="H38" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1706,16 +1725,16 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="H39" t="s">
-        <v>121</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1723,13 +1742,13 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="H40" s="5" t="s">
-        <v>123</v>
+        <v>45</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="H40" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1739,52 +1758,52 @@
       <c r="B41" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -1792,32 +1811,32 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>13</v>
       </c>
       <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,66 +1844,66 @@
         <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -1893,96 +1912,96 @@
       <c r="B55" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="58" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>68</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E63" t="s">
-        <v>86</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E64" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E65" t="s">
-        <v>83</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -1993,35 +2012,35 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D70">
         <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71">
         <v>4</v>
       </c>
       <c r="E71" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D72">
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2029,131 +2048,131 @@
         <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>150</v>
+      <c r="A78" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>106</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="G81">
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>105</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>107</v>
+        <v>233</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="G82">
         <v>2</v>
       </c>
       <c r="H82" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>159</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>158</v>
+        <v>150</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="G83">
         <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="G84">
         <v>4</v>
       </c>
       <c r="H84" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>151</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>109</v>
+        <v>142</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G85">
         <v>5</v>
       </c>
       <c r="H85" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>102</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="G86">
         <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>149</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>112</v>
+        <v>140</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="G87">
         <v>7</v>
       </c>
       <c r="H87" t="s">
-        <v>155</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -2161,98 +2180,98 @@
         <v>8</v>
       </c>
       <c r="H88" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G89">
         <v>9</v>
       </c>
       <c r="H89" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="C90" s="3"/>
       <c r="G90">
         <v>10</v>
       </c>
       <c r="H90" t="s">
-        <v>133</v>
+        <v>236</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>114</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="G91">
         <v>11</v>
       </c>
       <c r="H91" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>117</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="G92">
         <v>12</v>
       </c>
       <c r="H92" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>119</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="G93">
         <v>13</v>
       </c>
       <c r="H93" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>101</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>120</v>
+        <v>98</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="G94">
         <v>14</v>
       </c>
       <c r="H94" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>100</v>
-      </c>
-      <c r="C95" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="C95" s="3"/>
       <c r="G95">
         <v>15</v>
       </c>
       <c r="H95" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
@@ -2260,46 +2279,46 @@
         <v>16</v>
       </c>
       <c r="H96" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G97">
         <v>17</v>
       </c>
       <c r="H97" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>124</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="G98">
         <v>18</v>
       </c>
       <c r="H98" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>146</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="G99">
         <v>19</v>
       </c>
       <c r="H99" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -2307,367 +2326,394 @@
         <v>20</v>
       </c>
       <c r="H100" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>190</v>
+      <c r="A105" s="4" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
+      <c r="A106" s="4"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="H107" s="1"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>188</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>177</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>185</v>
+        <v>168</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>178</v>
-      </c>
-      <c r="D110" s="4" t="s">
-        <v>186</v>
+        <v>169</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>179</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>157</v>
+        <v>170</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>180</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>163</v>
+        <v>171</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>181</v>
-      </c>
-      <c r="D113" s="4" t="s">
-        <v>162</v>
+        <v>172</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>160</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>161</v>
+        <v>151</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>156</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>198</v>
+        <v>147</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E118" t="s">
-        <v>169</v>
+        <v>226</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
       </c>
       <c r="H118" t="s">
-        <v>240</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E119" t="s">
-        <v>164</v>
+        <v>173</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
       </c>
       <c r="H119" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>176</v>
-      </c>
-      <c r="C120" s="4"/>
+        <v>167</v>
+      </c>
+      <c r="C120" s="3"/>
       <c r="E120" t="s">
-        <v>165</v>
+        <v>183</v>
+      </c>
+      <c r="G120">
+        <v>3</v>
       </c>
       <c r="H120" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E121" t="s">
-        <v>166</v>
+        <v>174</v>
+      </c>
+      <c r="G121">
+        <v>4</v>
       </c>
       <c r="H121" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E122" t="s">
-        <v>167</v>
+        <v>184</v>
+      </c>
+      <c r="G122">
+        <v>5</v>
       </c>
       <c r="H122" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E123" t="s">
-        <v>168</v>
+        <v>185</v>
+      </c>
+      <c r="G123">
+        <v>6</v>
       </c>
       <c r="H123" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H124" s="6"/>
-      <c r="I124" s="6"/>
+      <c r="H124" s="5"/>
+      <c r="I124" s="5"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>192</v>
+      <c r="A125" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>238</v>
-      </c>
-      <c r="C133" s="4"/>
+        <v>224</v>
+      </c>
+      <c r="C133" s="3"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>240</v>
+      </c>
       <c r="B135" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B136" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>220</v>
+        <v>201</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>199</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>206</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>207</v>
+        <v>194</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>240</v>
+      </c>
       <c r="B141" t="s">
-        <v>203</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>205</v>
+        <v>192</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B142" t="s">
-        <v>201</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>202</v>
+        <v>190</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>217</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>218</v>
+        <v>204</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>216</v>
-      </c>
-      <c r="C146" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B147" t="s">
-        <v>223</v>
-      </c>
-      <c r="C147" s="4" t="s">
-        <v>225</v>
+        <v>209</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B148" t="s">
-        <v>215</v>
-      </c>
-      <c r="C148" s="4" t="s">
-        <v>244</v>
+        <v>202</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B149" t="s">
-        <v>221</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>222</v>
+        <v>207</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B150" t="s">
-        <v>226</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>227</v>
+        <v>212</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B151" t="s">
-        <v>228</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>229</v>
+        <v>214</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2675,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2683,10 +2729,10 @@
         <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>231</v>
-      </c>
-      <c r="C155" s="4" t="s">
-        <v>235</v>
+        <v>217</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2694,7 +2740,7 @@
         <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2702,19 +2748,24 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>230</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="C50:E50"/>
@@ -2731,11 +2782,6 @@
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>